<commit_message>
compiler: Allow binding outputs to methods with Object return type.
</commit_message>
<xml_diff>
--- a/components/system/src/test/data/org/formulacompiler/tutorials/TypeConversion.xlsx
+++ b/components/system/src/test/data/org/formulacompiler/tutorials/TypeConversion.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="123820"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="19320" windowHeight="15480"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="19320" windowHeight="15150"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Inputs</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>nulllong7</t>
+  </si>
+  <si>
+    <t>calcobject</t>
   </si>
 </sst>
 </file>
@@ -210,8 +213,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="171" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -614,7 +617,7 @@
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -639,7 +642,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="28" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="45">
@@ -976,11 +979,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -1523,6 +1524,14 @@
         <v>blabla</v>
       </c>
     </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>63</v>
+      </c>
+      <c r="B76">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>